<commit_message>
Make excel data nicer
</commit_message>
<xml_diff>
--- a/ExperimentalResults/GPSDataAll.xlsx
+++ b/ExperimentalResults/GPSDataAll.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tori\Documents\Master-Thesis\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tori\Documents\Master-Thesis\indoor-positioning-for-bim\ExperimentalResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79628CA-EF3D-48B2-BA3E-AB369876B2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB08D9D-1FBB-4B09-A5EB-0210EABFEF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33075" yWindow="4275" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Export" sheetId="1" r:id="rId1"/>
@@ -565,8 +565,8 @@
   <dimension ref="A1:Q116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O107" sqref="O107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4709,10 +4709,7 @@
       </c>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="O107" s="23">
-        <f>AVERAGE(O2:O105)</f>
-        <v>1917034.173076923</v>
-      </c>
+      <c r="O107" s="23"/>
     </row>
     <row r="115" spans="14:17" x14ac:dyDescent="0.2">
       <c r="N115" t="s">

</xml_diff>